<commit_message>
updated header to refer to new IG
</commit_message>
<xml_diff>
--- a/StructureDefinition-be-patient.xlsx
+++ b/StructureDefinition-be-patient.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3055" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3055" uniqueCount="435">
   <si>
     <t>Path</t>
   </si>
@@ -911,14 +911,11 @@
     <t>Patient.deceased[x]</t>
   </si>
   <si>
-    <t>boolean
-dateTime</t>
-  </si>
-  <si>
     <t>Indicates if the individual is deceased or not</t>
   </si>
   <si>
-    <t>Indicates if the individual is deceased or not.</t>
+    <t>Indicates if the individual is deceased or not.
+It is RECOMMENDED to include deceased information when applicable</t>
   </si>
   <si>
     <t>If there's no value in the instance, it means there is no statement on whether or not the individual is deceased. Most systems will interpret the absence of a value as a sign of the person being alive.</t>
@@ -7880,19 +7877,19 @@
         <v>52</v>
       </c>
       <c r="J56" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="K56" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="K56" t="s" s="2">
+      <c r="L56" t="s" s="2">
         <v>286</v>
       </c>
-      <c r="L56" t="s" s="2">
+      <c r="M56" t="s" s="2">
         <v>287</v>
       </c>
-      <c r="M56" t="s" s="2">
+      <c r="N56" t="s" s="2">
         <v>288</v>
-      </c>
-      <c r="N56" t="s" s="2">
-        <v>289</v>
       </c>
       <c r="O56" t="s" s="2">
         <v>44</v>
@@ -7956,7 +7953,7 @@
         <v>63</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="AK56" t="s" s="2">
         <v>112</v>
@@ -7965,7 +7962,7 @@
         <v>44</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AN56" t="s" s="2">
         <v>44</v>
@@ -7973,7 +7970,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7996,19 +7993,19 @@
         <v>44</v>
       </c>
       <c r="J57" t="s" s="2">
+        <v>292</v>
+      </c>
+      <c r="K57" t="s" s="2">
         <v>293</v>
       </c>
-      <c r="K57" t="s" s="2">
+      <c r="L57" t="s" s="2">
         <v>294</v>
       </c>
-      <c r="L57" t="s" s="2">
+      <c r="M57" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="M57" t="s" s="2">
+      <c r="N57" t="s" s="2">
         <v>296</v>
-      </c>
-      <c r="N57" t="s" s="2">
-        <v>297</v>
       </c>
       <c r="O57" t="s" s="2">
         <v>44</v>
@@ -8057,7 +8054,7 @@
         <v>44</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>42</v>
@@ -8072,16 +8069,16 @@
         <v>63</v>
       </c>
       <c r="AJ57" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="AK57" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL57" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM57" t="s" s="2">
         <v>298</v>
-      </c>
-      <c r="AK57" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AL57" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM57" t="s" s="2">
-        <v>299</v>
       </c>
       <c r="AN57" t="s" s="2">
         <v>44</v>
@@ -8089,7 +8086,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -8115,14 +8112,14 @@
         <v>129</v>
       </c>
       <c r="K58" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="L58" t="s" s="2">
         <v>301</v>
-      </c>
-      <c r="L58" t="s" s="2">
-        <v>302</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" t="s" s="2">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>44</v>
@@ -8151,7 +8148,7 @@
       </c>
       <c r="X58" s="2"/>
       <c r="Y58" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="Z58" t="s" s="2">
         <v>44</v>
@@ -8169,7 +8166,7 @@
         <v>44</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>42</v>
@@ -8184,16 +8181,16 @@
         <v>63</v>
       </c>
       <c r="AJ58" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="AK58" t="s" s="2">
         <v>305</v>
       </c>
-      <c r="AK58" t="s" s="2">
+      <c r="AL58" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM58" t="s" s="2">
         <v>306</v>
-      </c>
-      <c r="AL58" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM58" t="s" s="2">
-        <v>307</v>
       </c>
       <c r="AN58" t="s" s="2">
         <v>44</v>
@@ -8201,7 +8198,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8227,16 +8224,16 @@
         <v>219</v>
       </c>
       <c r="K59" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="L59" t="s" s="2">
         <v>309</v>
       </c>
-      <c r="L59" t="s" s="2">
+      <c r="M59" t="s" s="2">
         <v>310</v>
       </c>
-      <c r="M59" t="s" s="2">
+      <c r="N59" t="s" s="2">
         <v>311</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>312</v>
       </c>
       <c r="O59" t="s" s="2">
         <v>44</v>
@@ -8285,7 +8282,7 @@
         <v>44</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>42</v>
@@ -8300,7 +8297,7 @@
         <v>63</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="AK59" t="s" s="2">
         <v>112</v>
@@ -8309,7 +8306,7 @@
         <v>44</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>44</v>
@@ -8317,7 +8314,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8340,19 +8337,19 @@
         <v>44</v>
       </c>
       <c r="J60" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="K60" t="s" s="2">
         <v>316</v>
       </c>
-      <c r="K60" t="s" s="2">
+      <c r="L60" t="s" s="2">
         <v>317</v>
       </c>
-      <c r="L60" t="s" s="2">
+      <c r="M60" t="s" s="2">
         <v>318</v>
       </c>
-      <c r="M60" t="s" s="2">
+      <c r="N60" t="s" s="2">
         <v>319</v>
-      </c>
-      <c r="N60" t="s" s="2">
-        <v>320</v>
       </c>
       <c r="O60" t="s" s="2">
         <v>44</v>
@@ -8401,7 +8398,7 @@
         <v>44</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>42</v>
@@ -8416,7 +8413,7 @@
         <v>63</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AK60" t="s" s="2">
         <v>112</v>
@@ -8425,7 +8422,7 @@
         <v>44</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>44</v>
@@ -8433,7 +8430,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8456,19 +8453,19 @@
         <v>44</v>
       </c>
       <c r="J61" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="K61" t="s" s="2">
         <v>324</v>
       </c>
-      <c r="K61" t="s" s="2">
+      <c r="L61" t="s" s="2">
         <v>325</v>
       </c>
-      <c r="L61" t="s" s="2">
+      <c r="M61" t="s" s="2">
         <v>326</v>
       </c>
-      <c r="M61" t="s" s="2">
+      <c r="N61" t="s" s="2">
         <v>327</v>
-      </c>
-      <c r="N61" t="s" s="2">
-        <v>328</v>
       </c>
       <c r="O61" t="s" s="2">
         <v>44</v>
@@ -8517,7 +8514,7 @@
         <v>44</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>42</v>
@@ -8529,10 +8526,10 @@
         <v>44</v>
       </c>
       <c r="AI61" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="AJ61" t="s" s="2">
         <v>329</v>
-      </c>
-      <c r="AJ61" t="s" s="2">
-        <v>330</v>
       </c>
       <c r="AK61" t="s" s="2">
         <v>112</v>
@@ -8549,7 +8546,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8661,7 +8658,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8775,11 +8772,11 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" t="s" s="2">
@@ -8801,10 +8798,10 @@
         <v>96</v>
       </c>
       <c r="K64" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="L64" t="s" s="2">
         <v>335</v>
-      </c>
-      <c r="L64" t="s" s="2">
-        <v>336</v>
       </c>
       <c r="M64" t="s" s="2">
         <v>117</v>
@@ -8859,7 +8856,7 @@
         <v>44</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>42</v>
@@ -8891,7 +8888,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8917,14 +8914,14 @@
         <v>129</v>
       </c>
       <c r="K65" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="L65" t="s" s="2">
         <v>339</v>
-      </c>
-      <c r="L65" t="s" s="2">
-        <v>340</v>
       </c>
       <c r="M65" s="2"/>
       <c r="N65" t="s" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O65" t="s" s="2">
         <v>44</v>
@@ -8953,7 +8950,7 @@
       </c>
       <c r="X65" s="2"/>
       <c r="Y65" t="s" s="2">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="Z65" t="s" s="2">
         <v>44</v>
@@ -8971,7 +8968,7 @@
         <v>44</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>42</v>
@@ -8995,7 +8992,7 @@
         <v>44</v>
       </c>
       <c r="AM65" t="s" s="2">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="AN65" t="s" s="2">
         <v>44</v>
@@ -9003,7 +9000,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -9029,14 +9026,14 @@
         <v>228</v>
       </c>
       <c r="K66" t="s" s="2">
+        <v>344</v>
+      </c>
+      <c r="L66" t="s" s="2">
         <v>345</v>
-      </c>
-      <c r="L66" t="s" s="2">
-        <v>346</v>
       </c>
       <c r="M66" s="2"/>
       <c r="N66" t="s" s="2">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="O66" t="s" s="2">
         <v>44</v>
@@ -9085,7 +9082,7 @@
         <v>44</v>
       </c>
       <c r="AE66" t="s" s="2">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AF66" t="s" s="2">
         <v>42</v>
@@ -9109,7 +9106,7 @@
         <v>44</v>
       </c>
       <c r="AM66" t="s" s="2">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AN66" t="s" s="2">
         <v>44</v>
@@ -9117,7 +9114,7 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -9143,13 +9140,13 @@
         <v>237</v>
       </c>
       <c r="K67" t="s" s="2">
+        <v>349</v>
+      </c>
+      <c r="L67" t="s" s="2">
         <v>350</v>
       </c>
-      <c r="L67" t="s" s="2">
+      <c r="M67" t="s" s="2">
         <v>351</v>
-      </c>
-      <c r="M67" t="s" s="2">
-        <v>352</v>
       </c>
       <c r="N67" t="s" s="2">
         <v>241</v>
@@ -9201,7 +9198,7 @@
         <v>44</v>
       </c>
       <c r="AE67" t="s" s="2">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AF67" t="s" s="2">
         <v>42</v>
@@ -9225,7 +9222,7 @@
         <v>44</v>
       </c>
       <c r="AM67" t="s" s="2">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AN67" t="s" s="2">
         <v>44</v>
@@ -9233,7 +9230,7 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" t="s" s="2">
@@ -9259,14 +9256,14 @@
         <v>144</v>
       </c>
       <c r="K68" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="L68" t="s" s="2">
         <v>355</v>
-      </c>
-      <c r="L68" t="s" s="2">
-        <v>356</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="O68" t="s" s="2">
         <v>44</v>
@@ -9315,7 +9312,7 @@
         <v>44</v>
       </c>
       <c r="AE68" t="s" s="2">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AF68" t="s" s="2">
         <v>42</v>
@@ -9330,7 +9327,7 @@
         <v>63</v>
       </c>
       <c r="AJ68" t="s" s="2">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AK68" t="s" s="2">
         <v>112</v>
@@ -9339,7 +9336,7 @@
         <v>44</v>
       </c>
       <c r="AM68" t="s" s="2">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AN68" t="s" s="2">
         <v>44</v>
@@ -9347,7 +9344,7 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
@@ -9376,11 +9373,11 @@
         <v>246</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="M69" s="2"/>
       <c r="N69" t="s" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="O69" t="s" s="2">
         <v>44</v>
@@ -9429,7 +9426,7 @@
         <v>44</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>42</v>
@@ -9453,7 +9450,7 @@
         <v>44</v>
       </c>
       <c r="AM69" t="s" s="2">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AN69" t="s" s="2">
         <v>44</v>
@@ -9461,7 +9458,7 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
@@ -9487,14 +9484,14 @@
         <v>211</v>
       </c>
       <c r="K70" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="L70" t="s" s="2">
         <v>365</v>
-      </c>
-      <c r="L70" t="s" s="2">
-        <v>366</v>
       </c>
       <c r="M70" s="2"/>
       <c r="N70" t="s" s="2">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="O70" t="s" s="2">
         <v>44</v>
@@ -9543,7 +9540,7 @@
         <v>44</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>42</v>
@@ -9552,13 +9549,13 @@
         <v>51</v>
       </c>
       <c r="AH70" t="s" s="2">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AI70" t="s" s="2">
         <v>63</v>
       </c>
       <c r="AJ70" t="s" s="2">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AK70" t="s" s="2">
         <v>112</v>
@@ -9567,7 +9564,7 @@
         <v>44</v>
       </c>
       <c r="AM70" t="s" s="2">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AN70" t="s" s="2">
         <v>44</v>
@@ -9575,7 +9572,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9601,10 +9598,10 @@
         <v>134</v>
       </c>
       <c r="K71" t="s" s="2">
+        <v>371</v>
+      </c>
+      <c r="L71" t="s" s="2">
         <v>372</v>
-      </c>
-      <c r="L71" t="s" s="2">
-        <v>373</v>
       </c>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -9655,7 +9652,7 @@
         <v>44</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>42</v>
@@ -9670,7 +9667,7 @@
         <v>63</v>
       </c>
       <c r="AJ71" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AK71" t="s" s="2">
         <v>112</v>
@@ -9687,7 +9684,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9710,19 +9707,19 @@
         <v>44</v>
       </c>
       <c r="J72" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K72" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="L72" t="s" s="2">
         <v>376</v>
       </c>
-      <c r="L72" t="s" s="2">
+      <c r="M72" t="s" s="2">
         <v>377</v>
       </c>
-      <c r="M72" t="s" s="2">
+      <c r="N72" t="s" s="2">
         <v>378</v>
-      </c>
-      <c r="N72" t="s" s="2">
-        <v>379</v>
       </c>
       <c r="O72" t="s" s="2">
         <v>44</v>
@@ -9771,7 +9768,7 @@
         <v>44</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>42</v>
@@ -9786,10 +9783,10 @@
         <v>63</v>
       </c>
       <c r="AJ72" t="s" s="2">
+        <v>379</v>
+      </c>
+      <c r="AK72" t="s" s="2">
         <v>380</v>
-      </c>
-      <c r="AK72" t="s" s="2">
-        <v>381</v>
       </c>
       <c r="AL72" t="s" s="2">
         <v>44</v>
@@ -9803,7 +9800,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -9915,7 +9912,7 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -10029,11 +10026,11 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" t="s" s="2">
@@ -10055,10 +10052,10 @@
         <v>96</v>
       </c>
       <c r="K75" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="L75" t="s" s="2">
         <v>335</v>
-      </c>
-      <c r="L75" t="s" s="2">
-        <v>336</v>
       </c>
       <c r="M75" t="s" s="2">
         <v>117</v>
@@ -10113,7 +10110,7 @@
         <v>44</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>42</v>
@@ -10145,7 +10142,7 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -10171,16 +10168,16 @@
         <v>129</v>
       </c>
       <c r="K76" t="s" s="2">
+        <v>385</v>
+      </c>
+      <c r="L76" t="s" s="2">
         <v>386</v>
       </c>
-      <c r="L76" t="s" s="2">
+      <c r="M76" t="s" s="2">
         <v>387</v>
       </c>
-      <c r="M76" t="s" s="2">
+      <c r="N76" t="s" s="2">
         <v>388</v>
-      </c>
-      <c r="N76" t="s" s="2">
-        <v>389</v>
       </c>
       <c r="O76" t="s" s="2">
         <v>44</v>
@@ -10229,7 +10226,7 @@
         <v>44</v>
       </c>
       <c r="AE76" t="s" s="2">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AF76" t="s" s="2">
         <v>51</v>
@@ -10244,16 +10241,16 @@
         <v>63</v>
       </c>
       <c r="AJ76" t="s" s="2">
+        <v>389</v>
+      </c>
+      <c r="AK76" t="s" s="2">
         <v>390</v>
       </c>
-      <c r="AK76" t="s" s="2">
+      <c r="AL76" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM76" t="s" s="2">
         <v>391</v>
-      </c>
-      <c r="AL76" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM76" t="s" s="2">
-        <v>392</v>
       </c>
       <c r="AN76" t="s" s="2">
         <v>44</v>
@@ -10261,7 +10258,7 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -10287,16 +10284,16 @@
         <v>219</v>
       </c>
       <c r="K77" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="L77" t="s" s="2">
         <v>394</v>
       </c>
-      <c r="L77" t="s" s="2">
+      <c r="M77" t="s" s="2">
         <v>395</v>
       </c>
-      <c r="M77" t="s" s="2">
+      <c r="N77" t="s" s="2">
         <v>396</v>
-      </c>
-      <c r="N77" t="s" s="2">
-        <v>397</v>
       </c>
       <c r="O77" t="s" s="2">
         <v>44</v>
@@ -10345,7 +10342,7 @@
         <v>44</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>42</v>
@@ -10360,16 +10357,16 @@
         <v>63</v>
       </c>
       <c r="AJ77" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="AK77" t="s" s="2">
         <v>398</v>
       </c>
-      <c r="AK77" t="s" s="2">
+      <c r="AL77" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AM77" t="s" s="2">
         <v>399</v>
-      </c>
-      <c r="AL77" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AM77" t="s" s="2">
-        <v>400</v>
       </c>
       <c r="AN77" t="s" s="2">
         <v>44</v>
@@ -10377,11 +10374,11 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" t="s" s="2">
@@ -10400,16 +10397,16 @@
         <v>44</v>
       </c>
       <c r="J78" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="K78" t="s" s="2">
         <v>403</v>
       </c>
-      <c r="K78" t="s" s="2">
+      <c r="L78" t="s" s="2">
         <v>404</v>
       </c>
-      <c r="L78" t="s" s="2">
+      <c r="M78" t="s" s="2">
         <v>405</v>
-      </c>
-      <c r="M78" t="s" s="2">
-        <v>406</v>
       </c>
       <c r="N78" s="2"/>
       <c r="O78" t="s" s="2">
@@ -10459,7 +10456,7 @@
         <v>44</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>42</v>
@@ -10474,7 +10471,7 @@
         <v>63</v>
       </c>
       <c r="AJ78" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AK78" t="s" s="2">
         <v>112</v>
@@ -10483,7 +10480,7 @@
         <v>44</v>
       </c>
       <c r="AM78" t="s" s="2">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AN78" t="s" s="2">
         <v>44</v>
@@ -10491,7 +10488,7 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -10514,19 +10511,19 @@
         <v>52</v>
       </c>
       <c r="J79" t="s" s="2">
+        <v>409</v>
+      </c>
+      <c r="K79" t="s" s="2">
         <v>410</v>
       </c>
-      <c r="K79" t="s" s="2">
+      <c r="L79" t="s" s="2">
         <v>411</v>
       </c>
-      <c r="L79" t="s" s="2">
+      <c r="M79" t="s" s="2">
         <v>412</v>
       </c>
-      <c r="M79" t="s" s="2">
+      <c r="N79" t="s" s="2">
         <v>413</v>
-      </c>
-      <c r="N79" t="s" s="2">
-        <v>414</v>
       </c>
       <c r="O79" t="s" s="2">
         <v>44</v>
@@ -10575,7 +10572,7 @@
         <v>44</v>
       </c>
       <c r="AE79" t="s" s="2">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AF79" t="s" s="2">
         <v>42</v>
@@ -10590,10 +10587,10 @@
         <v>63</v>
       </c>
       <c r="AJ79" t="s" s="2">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AK79" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AL79" t="s" s="2">
         <v>44</v>
@@ -10607,7 +10604,7 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10630,19 +10627,19 @@
         <v>52</v>
       </c>
       <c r="J80" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K80" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="L80" t="s" s="2">
         <v>417</v>
       </c>
-      <c r="L80" t="s" s="2">
+      <c r="M80" t="s" s="2">
         <v>418</v>
       </c>
-      <c r="M80" t="s" s="2">
+      <c r="N80" t="s" s="2">
         <v>419</v>
-      </c>
-      <c r="N80" t="s" s="2">
-        <v>420</v>
       </c>
       <c r="O80" t="s" s="2">
         <v>44</v>
@@ -10691,7 +10688,7 @@
         <v>44</v>
       </c>
       <c r="AE80" t="s" s="2">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="AF80" t="s" s="2">
         <v>42</v>
@@ -10706,7 +10703,7 @@
         <v>63</v>
       </c>
       <c r="AJ80" t="s" s="2">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AK80" t="s" s="2">
         <v>112</v>
@@ -10723,7 +10720,7 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" t="s" s="2">
@@ -10835,7 +10832,7 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
@@ -10949,11 +10946,11 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" t="s" s="2">
@@ -10975,10 +10972,10 @@
         <v>96</v>
       </c>
       <c r="K83" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="L83" t="s" s="2">
         <v>335</v>
-      </c>
-      <c r="L83" t="s" s="2">
-        <v>336</v>
       </c>
       <c r="M83" t="s" s="2">
         <v>117</v>
@@ -11033,7 +11030,7 @@
         <v>44</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AF83" t="s" s="2">
         <v>42</v>
@@ -11065,7 +11062,7 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
@@ -11088,16 +11085,16 @@
         <v>52</v>
       </c>
       <c r="J84" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="K84" t="s" s="2">
         <v>426</v>
       </c>
-      <c r="K84" t="s" s="2">
+      <c r="L84" t="s" s="2">
         <v>427</v>
       </c>
-      <c r="L84" t="s" s="2">
+      <c r="M84" t="s" s="2">
         <v>428</v>
-      </c>
-      <c r="M84" t="s" s="2">
-        <v>429</v>
       </c>
       <c r="N84" s="2"/>
       <c r="O84" t="s" s="2">
@@ -11147,7 +11144,7 @@
         <v>44</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>51</v>
@@ -11171,7 +11168,7 @@
         <v>44</v>
       </c>
       <c r="AM84" t="s" s="2">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="AN84" t="s" s="2">
         <v>44</v>
@@ -11179,7 +11176,7 @@
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
@@ -11205,10 +11202,10 @@
         <v>71</v>
       </c>
       <c r="K85" t="s" s="2">
+        <v>431</v>
+      </c>
+      <c r="L85" t="s" s="2">
         <v>432</v>
-      </c>
-      <c r="L85" t="s" s="2">
-        <v>433</v>
       </c>
       <c r="M85" s="2"/>
       <c r="N85" s="2"/>
@@ -11238,11 +11235,11 @@
         <v>171</v>
       </c>
       <c r="X85" t="s" s="2">
+        <v>432</v>
+      </c>
+      <c r="Y85" t="s" s="2">
         <v>433</v>
       </c>
-      <c r="Y85" t="s" s="2">
-        <v>434</v>
-      </c>
       <c r="Z85" t="s" s="2">
         <v>44</v>
       </c>
@@ -11259,7 +11256,7 @@
         <v>44</v>
       </c>
       <c r="AE85" t="s" s="2">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="AF85" t="s" s="2">
         <v>51</v>
@@ -11274,7 +11271,7 @@
         <v>63</v>
       </c>
       <c r="AJ85" t="s" s="2">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="AK85" t="s" s="2">
         <v>112</v>

</xml_diff>